<commit_message>
latest push (minor changes)
</commit_message>
<xml_diff>
--- a/data/all_roi_df.xlsx
+++ b/data/all_roi_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rweberla/flybrain-clustering-rhessa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rweberla/Documents/GitHub/oviIN-inputs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB150C7-BC18-304B-80D2-7EFE641D735B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181BA328-C2E0-5E4D-89CA-184F6D2DB8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="1360" windowWidth="22500" windowHeight="22020" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
+    <workbookView xWindow="41200" yWindow="12940" windowWidth="22500" windowHeight="22020" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:H231"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>